<commit_message>
update bolew and sdcol
</commit_message>
<xml_diff>
--- a/models/bolser-lewis/source/bolser-lewis.xlsx
+++ b/models/bolser-lewis/source/bolser-lewis.xlsx
@@ -866,25 +866,25 @@
     <t>neuron-3</t>
   </si>
   <si>
-    <t>Soma in 265 (bolew)</t>
+    <t>Soma in 265 - Phrenic nucleus of C4 (bolew)</t>
   </si>
   <si>
     <t>neuron-4</t>
   </si>
   <si>
-    <t>Soma in 266 (bolew)</t>
+    <t>Soma in 266 - Phrenic nucleus of C5 (bolew)</t>
   </si>
   <si>
     <t>neuron-5</t>
   </si>
   <si>
-    <t>Soma in 262 (bolew)</t>
+    <t>Soma in 262 - Nucleus tractus solitarius(bolew)</t>
   </si>
   <si>
     <t>neuron-6</t>
   </si>
   <si>
-    <t>Soma in 264 (bolew)</t>
+    <t>Soma in 264 - Rostral ventrolateral medulla(bolew)</t>
   </si>
   <si>
     <t>neuron-7</t>
@@ -893,7 +893,7 @@
     <t>soma249_1</t>
   </si>
   <si>
-    <t>Soma in 249 (1) (bolew)</t>
+    <t>Soma in 249 (1) - Nodose ganglion of the Vagus nerve(bolew)</t>
   </si>
   <si>
     <t>neuron-8</t>
@@ -902,7 +902,7 @@
     <t>soma249_2</t>
   </si>
   <si>
-    <t>Soma in 249 (2) (bolew)</t>
+    <t>Soma in 249 (2) - Nodose ganglion of the Vagus nerve(bolew)</t>
   </si>
   <si>
     <t>neuron-9</t>
@@ -911,7 +911,7 @@
     <t>soma249_3</t>
   </si>
   <si>
-    <t>Soma in 249 (3) (bolew)</t>
+    <t>Soma in 249 (3) - Nodose ganglion of the Vagus nerve(bolew)</t>
   </si>
   <si>
     <t>neuron-10</t>
@@ -920,7 +920,7 @@
     <t>soma248_1</t>
   </si>
   <si>
-    <t>Soma in 248 (1) (bolew)</t>
+    <t>Soma in 248 (1) - Petrosal ganglion of the Glossopharyngeal nerve(bolew)</t>
   </si>
   <si>
     <t>neuron-11</t>
@@ -929,7 +929,7 @@
     <t>soma248_2</t>
   </si>
   <si>
-    <t>Soma in 248 (2) (bolew)</t>
+    <t>Soma in 248 (2) - Petrosal ganglion of the Glossopharyngeal nerve(bolew)</t>
   </si>
   <si>
     <t>neuron-12</t>
@@ -7676,146 +7676,6 @@
         <v>322</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="24"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="58"/>
-      <c r="D116" s="25"/>
-      <c r="E116" s="59"/>
-      <c r="F116" s="25"/>
-      <c r="G116" s="25"/>
-      <c r="H116" s="60"/>
-      <c r="I116" s="61"/>
-      <c r="J116" s="22"/>
-      <c r="M116" s="16"/>
-      <c r="O116" s="17"/>
-    </row>
-    <row r="117">
-      <c r="A117" s="24"/>
-      <c r="B117" s="8"/>
-      <c r="C117" s="58"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="59"/>
-      <c r="F117" s="25"/>
-      <c r="G117" s="25"/>
-      <c r="H117" s="60"/>
-      <c r="I117" s="61"/>
-      <c r="J117" s="22"/>
-      <c r="M117" s="16"/>
-      <c r="O117" s="17"/>
-    </row>
-    <row r="118">
-      <c r="A118" s="24"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="58"/>
-      <c r="D118" s="25"/>
-      <c r="E118" s="59"/>
-      <c r="F118" s="25"/>
-      <c r="G118" s="25"/>
-      <c r="H118" s="60"/>
-      <c r="I118" s="61"/>
-      <c r="J118" s="22"/>
-      <c r="M118" s="16"/>
-      <c r="O118" s="17"/>
-    </row>
-    <row r="119">
-      <c r="A119" s="24"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="58"/>
-      <c r="D119" s="25"/>
-      <c r="E119" s="59"/>
-      <c r="F119" s="25"/>
-      <c r="G119" s="25"/>
-      <c r="H119" s="60"/>
-      <c r="I119" s="61"/>
-      <c r="J119" s="22"/>
-      <c r="M119" s="16"/>
-      <c r="O119" s="17"/>
-    </row>
-    <row r="120">
-      <c r="A120" s="24"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="58"/>
-      <c r="D120" s="25"/>
-      <c r="E120" s="59"/>
-      <c r="F120" s="25"/>
-      <c r="G120" s="25"/>
-      <c r="H120" s="60"/>
-      <c r="I120" s="61"/>
-      <c r="J120" s="22"/>
-      <c r="M120" s="16"/>
-      <c r="O120" s="17"/>
-    </row>
-    <row r="121">
-      <c r="A121" s="24"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="58"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="59"/>
-      <c r="F121" s="25"/>
-      <c r="G121" s="25"/>
-      <c r="H121" s="60"/>
-      <c r="I121" s="61"/>
-      <c r="J121" s="22"/>
-      <c r="M121" s="16"/>
-      <c r="O121" s="17"/>
-    </row>
-    <row r="122">
-      <c r="A122" s="24"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="58"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="59"/>
-      <c r="F122" s="25"/>
-      <c r="G122" s="25"/>
-      <c r="H122" s="60"/>
-      <c r="I122" s="61"/>
-      <c r="J122" s="22"/>
-      <c r="M122" s="16"/>
-      <c r="O122" s="17"/>
-    </row>
-    <row r="123">
-      <c r="A123" s="24"/>
-      <c r="B123" s="8"/>
-      <c r="C123" s="58"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="59"/>
-      <c r="F123" s="25"/>
-      <c r="G123" s="25"/>
-      <c r="H123" s="60"/>
-      <c r="I123" s="61"/>
-      <c r="J123" s="22"/>
-      <c r="M123" s="16"/>
-      <c r="O123" s="17"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="24"/>
-      <c r="B124" s="8"/>
-      <c r="C124" s="58"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="59"/>
-      <c r="F124" s="25"/>
-      <c r="G124" s="25"/>
-      <c r="H124" s="60"/>
-      <c r="I124" s="61"/>
-      <c r="J124" s="22"/>
-      <c r="M124" s="16"/>
-      <c r="O124" s="17"/>
-    </row>
-    <row r="125">
-      <c r="A125" s="24"/>
-      <c r="B125" s="8"/>
-      <c r="C125" s="58"/>
-      <c r="D125" s="25"/>
-      <c r="E125" s="59"/>
-      <c r="F125" s="25"/>
-      <c r="G125" s="25"/>
-      <c r="H125" s="60"/>
-      <c r="I125" s="61"/>
-      <c r="J125" s="22"/>
-      <c r="M125" s="16"/>
-      <c r="O125" s="17"/>
-    </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>